<commit_message>
fix scroll add enter event to cell
</commit_message>
<xml_diff>
--- a/documents/TEST.xlsx
+++ b/documents/TEST.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N5000"/>
+  <dimension ref="A1:EA6000"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -415,6 +415,12 @@
       <c r="N1" t="b">
         <v>0</v>
       </c>
+      <c r="DA1" t="str">
+        <v>cbvcbcv</v>
+      </c>
+      <c r="EA1" t="str">
+        <v>vsdvs</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2">
@@ -424,7 +430,7 @@
         <v>February</v>
       </c>
       <c r="C2">
-        <v>1993</v>
+        <v>1993cscascascsa</v>
       </c>
     </row>
     <row r="3">
@@ -459,6 +465,9 @@
       <c r="C5">
         <v>1996</v>
       </c>
+      <c r="DA5" t="str">
+        <v>cvbcv</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -469,6 +478,9 @@
       </c>
       <c r="C6">
         <v>1997</v>
+      </c>
+      <c r="EA6" t="str">
+        <v>vsdvsd</v>
       </c>
     </row>
     <row r="7">
@@ -527,6 +539,9 @@
       <c r="C11">
         <v>2002</v>
       </c>
+      <c r="EA11" t="str">
+        <v>sdvsd</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12">
@@ -538,6 +553,9 @@
       <c r="C12">
         <v>2003</v>
       </c>
+      <c r="DA12" t="str">
+        <v>cvbcv</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13">
@@ -604,6 +622,9 @@
       <c r="C18">
         <v>2009</v>
       </c>
+      <c r="DA18" t="str">
+        <v>cvbcvb</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19">
@@ -615,6 +636,9 @@
       <c r="C19">
         <v>2010</v>
       </c>
+      <c r="EA19" t="str">
+        <v>sdvsdv</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20">
@@ -661,6 +685,16 @@
         <v>test</v>
       </c>
     </row>
+    <row r="23">
+      <c r="DA23" t="str">
+        <v>vbcvbc</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="EA24" t="str">
+        <v>vsdvs</v>
+      </c>
+    </row>
     <row r="25">
       <c r="A25" t="str">
         <v>test</v>
@@ -670,6 +704,26 @@
       </c>
       <c r="C25" t="str">
         <v>test</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="DA28" t="str">
+        <v>bcvb</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="EA30" t="str">
+        <v>sdv</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="DA32" t="str">
+        <v>fdfbd</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="EA33" t="str">
+        <v>v</v>
       </c>
     </row>
     <row r="5000">
@@ -695,10 +749,44 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5999">
+      <c r="M5999" t="str">
+        <v>sdf</v>
+      </c>
+    </row>
+    <row r="6000">
+      <c r="A6000">
+        <v>123</v>
+      </c>
+      <c r="B6000" t="str">
+        <v>sdfs</v>
+      </c>
+      <c r="D6000" t="str">
+        <v>fsdfsd</v>
+      </c>
+      <c r="G6000" t="str">
+        <v>sdfsdf</v>
+      </c>
+      <c r="J6000" t="str">
+        <v>sdfsd</v>
+      </c>
+      <c r="O6000" t="str">
+        <v>sdfsdf</v>
+      </c>
+      <c r="R6000" t="str">
+        <v>dfsdfsd</v>
+      </c>
+      <c r="V6000" t="str">
+        <v>sdfds</v>
+      </c>
+      <c r="DA6000" t="str">
+        <v>sdfsdfsdfs</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N5000"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:EA6000"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>